<commit_message>
working on displaying fase selection
</commit_message>
<xml_diff>
--- a/mockup/answers.xlsx
+++ b/mockup/answers.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://surf.sharepoint.com/sites/m365-WRKGTOA-team/Gedeelde documenten/Projecten/Toetsweb/MockUp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shklinkenberg/GitHub/toetsweb/mockup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{09B1600C-D21A-9A4A-AE42-8F0759CA44F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8043288F-9348-9741-A96E-DF3B806EAC61}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88844689-FFBF-3648-B668-5F1E7F6E9BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="-19200" windowWidth="28040" windowHeight="17440" xr2:uid="{E3918505-BA42-FE4E-8C71-7290711BE4A3}"/>
+    <workbookView xWindow="-4040" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{E3918505-BA42-FE4E-8C71-7290711BE4A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="answerOptions" sheetId="1" r:id="rId1"/>
+    <sheet name="fase" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="87">
   <si>
     <t>entiteit.id</t>
   </si>
@@ -263,6 +264,39 @@
   </si>
   <si>
     <t>Toetsbekwaamheid</t>
+  </si>
+  <si>
+    <t>Activiteit-georiënteerde fase</t>
+  </si>
+  <si>
+    <t>Proces-georiënteerde fase</t>
+  </si>
+  <si>
+    <t>Systeem-georiënteerde fase</t>
+  </si>
+  <si>
+    <t>Keten-georiënteerde fase</t>
+  </si>
+  <si>
+    <t>kwaliteitscriteriaScore</t>
+  </si>
+  <si>
+    <t>ontwerpScore</t>
+  </si>
+  <si>
+    <t>borgingScore</t>
+  </si>
+  <si>
+    <t>faseSelectId</t>
+  </si>
+  <si>
+    <t>faseId</t>
+  </si>
+  <si>
+    <t>faseNaam</t>
+  </si>
+  <si>
+    <t>faseBeschrijving</t>
   </si>
 </sst>
 </file>
@@ -616,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F34DC85-FA6C-EF45-B4E2-5DD82D3D924B}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView zoomScale="209" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2045,4 +2079,1393 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C3C063-7ABA-BB44-823D-914C57C2E060}">
+  <dimension ref="A1:G65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT(A2:C2)</f>
+        <v>111</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D65" si="0">_xlfn.CONCAT(A3:C3)</f>
+        <v>112</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>211</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>221</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>141</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>411</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>213</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>222</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>312</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>214</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>223</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>241</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>313</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>322</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>331</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>412</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>421</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>314</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>332</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>341</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>413</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>422</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>431</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>234</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>414</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>432</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>424</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>442</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>333</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>343</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>433</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>434</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+      <c r="F65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>